<commit_message>
added third test, refactoring done for separate Dataprovider and action s=on pages are moved to BaseTest class
</commit_message>
<xml_diff>
--- a/src/test/resources/excelsheet/TestData.xlsx
+++ b/src/test/resources/excelsheet/TestData.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF725BA-6C21-436D-A50F-9FC18FA252F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C4B2BB-17E9-4B43-974D-ABFFD8306932}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="testData" sheetId="1" r:id="rId1"/>
+    <sheet name="createCustomerData" sheetId="1" r:id="rId1"/>
+    <sheet name="openAccountData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>firstName</t>
   </si>
@@ -44,6 +45,42 @@
   </si>
   <si>
     <t>623001</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>wick</t>
+  </si>
+  <si>
+    <t>Malena</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>650001</t>
+  </si>
+  <si>
+    <t>632102</t>
+  </si>
+  <si>
+    <t>customerName</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>alert</t>
+  </si>
+  <si>
+    <t>Account created successfully</t>
   </si>
 </sst>
 </file>
@@ -362,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,6 +438,75 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FD1AA7-203C-4B9A-A549-48A6630C0602}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>